<commit_message>
监察委+公文 Signed-off-by: fengjinliang <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/sydw/2020上/考点/1-法律法规.xlsx
+++ b/sydw/2020上/考点/1-法律法规.xlsx
@@ -4,24 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="19200" windowHeight="7130" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="宪法" sheetId="1" r:id="rId2"/>
     <sheet name="事业单位公开招聘人员暂行规定" sheetId="2" r:id="rId3"/>
+    <sheet name="监察" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="336">
   <si>
     <t>宪法</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>1.中华人民共和国</t>
     </r>
     <r>
@@ -36,6 +43,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>2.中华人民共和国</t>
     </r>
     <r>
@@ -50,6 +63,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>3.中华人民共和国</t>
     </r>
     <r>
@@ -64,6 +83,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>4.中华人民共和国</t>
     </r>
     <r>
@@ -78,6 +103,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>5.中华人民共和国</t>
     </r>
     <r>
@@ -92,6 +123,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>6.中华人民共和国</t>
     </r>
     <r>
@@ -106,6 +143,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>7.中华人民共和国</t>
     </r>
     <r>
@@ -126,6 +169,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>10.中华人民共和国</t>
     </r>
     <r>
@@ -143,6 +192,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>12.中华人民共和国</t>
     </r>
     <r>
@@ -157,6 +212,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>13.中华人民共和国</t>
     </r>
     <r>
@@ -171,6 +232,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>14.中华人民共和国</t>
     </r>
     <r>
@@ -999,6 +1066,153 @@
   <si>
     <t>坚持德才兼备的用人标准，贯彻公开，公平，竞争，择优的原则</t>
   </si>
+  <si>
+    <t>监察委员会</t>
+  </si>
+  <si>
+    <t>性质</t>
+  </si>
+  <si>
+    <t>监察机关</t>
+  </si>
+  <si>
+    <t>设置</t>
+  </si>
+  <si>
+    <t>国家监察委员会</t>
+  </si>
+  <si>
+    <t>对全人大和全人常负责</t>
+  </si>
+  <si>
+    <t>国家监察委主任连续任职不超过2届</t>
+  </si>
+  <si>
+    <t>地方监察委员会</t>
+  </si>
+  <si>
+    <t>对地方权力机关和上一级监察委负责</t>
+  </si>
+  <si>
+    <t>省、市、县</t>
+  </si>
+  <si>
+    <t>与人大</t>
+  </si>
+  <si>
+    <t>人大人常监督监察委员会工作</t>
+  </si>
+  <si>
+    <t>人大选举本级监察委员会主任</t>
+  </si>
+  <si>
+    <t>人大根据监察主任提请，任免监察委员会副主任、委员</t>
+  </si>
+  <si>
+    <t>职权</t>
+  </si>
+  <si>
+    <t>监督、调查、处置</t>
+  </si>
+  <si>
+    <t>独立行使职权</t>
+  </si>
+  <si>
+    <t>与审判、检察、执法相互配合，相互制约</t>
+  </si>
+  <si>
+    <t>事实为根据，法律为准绳</t>
+  </si>
+  <si>
+    <t>适用法律平等，保障合法权益</t>
+  </si>
+  <si>
+    <t>权责对等，严格监督</t>
+  </si>
+  <si>
+    <t>惩教结合，宽严相济</t>
+  </si>
+  <si>
+    <t>管辖</t>
+  </si>
+  <si>
+    <t>一般管辖</t>
+  </si>
+  <si>
+    <t>上下级</t>
+  </si>
+  <si>
+    <t>上级可管辖下级事项，可将事项制定给下级</t>
+  </si>
+  <si>
+    <t>下级可以报请上级管辖，下级有争议找上级解决</t>
+  </si>
+  <si>
+    <t>回避</t>
+  </si>
+  <si>
+    <t>是监察对象或者检举人的近亲属：证人</t>
+  </si>
+  <si>
+    <t>本人或者近亲属与监察事项有利害关系：其他</t>
+  </si>
+  <si>
+    <t>留置</t>
+  </si>
+  <si>
+    <t>适用条件</t>
+  </si>
+  <si>
+    <t>严重：需进一步调查：符合以下</t>
+  </si>
+  <si>
+    <t>重大、复杂</t>
+  </si>
+  <si>
+    <t>逃跑、自杀</t>
+  </si>
+  <si>
+    <t>串供、伪造、毁灭、隐匿证据</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>行贿、共同职务犯罪的人</t>
+  </si>
+  <si>
+    <t>程序</t>
+  </si>
+  <si>
+    <t>集体研究决定，留置后一般24小时内通知</t>
+  </si>
+  <si>
+    <t>市县报上一级批准，省报上一级备案</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>一般3个月，最长6个月</t>
+  </si>
+  <si>
+    <t>折抵：折抵管制2日，折抵拘役/有期1日</t>
+  </si>
+  <si>
+    <t>处置</t>
+  </si>
+  <si>
+    <t>谈话提醒、政务处分、移送起诉、问责、监察建议</t>
+  </si>
+  <si>
+    <t>救济：复审(1个月申请，1个月决定)--复核(1个月申请，2个月决定)</t>
+  </si>
+  <si>
+    <t>监督</t>
+  </si>
+  <si>
+    <t>权利机关的监督、社会监督、自我监督</t>
+  </si>
 </sst>
 </file>
 
@@ -1006,9 +1220,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1037,77 +1251,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1127,6 +1275,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
@@ -1134,8 +1305,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1143,7 +1322,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1166,18 +1359,39 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1187,12 +1401,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.05"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1208,7 +1428,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1220,37 +1524,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1266,134 +1612,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1405,6 +1625,43 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1461,9 +1718,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1472,19 +1727,24 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color auto="1"/>
-      </right>
-      <top style="thin">
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
-      </top>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1502,51 +1762,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1561,21 +1779,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1596,6 +1799,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1606,16 +1833,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1624,145 +1875,145 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1781,8 +2032,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1790,16 +2041,65 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1808,10 +2108,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1907,7 +2204,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371600" y="809625"/>
+          <a:off x="1371600" y="806450"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1948,7 +2245,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371600" y="4791075"/>
+          <a:off x="1371600" y="4787900"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1989,7 +2286,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371600" y="7515225"/>
+          <a:off x="1371600" y="7512050"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2030,7 +2327,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1371600" y="17364075"/>
+          <a:off x="1371600" y="17360900"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2307,692 +2604,692 @@
   <sheetPr/>
   <dimension ref="B2:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
   <cols>
     <col min="3" max="3" width="115.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="16.5" spans="2:3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="35" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="2:3">
-      <c r="B3" s="19"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="2:3">
-      <c r="B4" s="19"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="35" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" ht="16.5" spans="2:3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="36" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="2:3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="35" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="16.5" spans="2:3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" ht="16.5" spans="2:3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="16.5" spans="2:3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="18" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="2:3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="35" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" ht="16.5" spans="2:3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="35" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" ht="16.5" spans="2:3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="35" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" ht="16.5" spans="2:3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="35" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" ht="16.5" spans="2:3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="35" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" ht="16.5" spans="2:3">
-      <c r="B15" s="19"/>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" ht="16.5" spans="2:3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="18" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="35" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" ht="16.5" spans="2:3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="18" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="35" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" ht="16.5" spans="2:3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="35" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" ht="16.5" spans="2:3">
-      <c r="B19" s="19"/>
-      <c r="C19" s="18" t="s">
+      <c r="B19" s="34"/>
+      <c r="C19" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" ht="16.5" spans="2:3">
-      <c r="B20" s="19"/>
-      <c r="C20" s="18" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="35" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="21" ht="16.5" spans="2:3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="35" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" ht="16.5" spans="2:3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="35" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" ht="16.5" spans="2:3">
-      <c r="B23" s="21"/>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="37"/>
+      <c r="C23" s="35" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" ht="16.5" spans="2:3">
-      <c r="B24" s="21"/>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="37"/>
+      <c r="C24" s="35" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" ht="16.5" spans="2:3">
-      <c r="B25" s="21"/>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="37"/>
+      <c r="C25" s="35" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" ht="16.5" spans="2:3">
-      <c r="B26" s="21"/>
-      <c r="C26" s="18" t="s">
+      <c r="B26" s="37"/>
+      <c r="C26" s="35" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" ht="16.5" spans="2:3">
-      <c r="B27" s="21"/>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="37"/>
+      <c r="C27" s="35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" ht="16.5" spans="2:3">
-      <c r="B28" s="21"/>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="37"/>
+      <c r="C28" s="35" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" ht="16.5" spans="2:3">
-      <c r="B29" s="21"/>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="37"/>
+      <c r="C29" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" ht="16.5" spans="2:3">
-      <c r="B30" s="21"/>
-      <c r="C30" s="18" t="s">
+      <c r="B30" s="37"/>
+      <c r="C30" s="35" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" ht="16.5" spans="2:3">
-      <c r="B31" s="21"/>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="37"/>
+      <c r="C31" s="35" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" ht="16.5" spans="2:3">
-      <c r="B32" s="21"/>
-      <c r="C32" s="18" t="s">
+      <c r="B32" s="37"/>
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" ht="16.5" spans="2:3">
-      <c r="B33" s="21"/>
-      <c r="C33" s="18" t="s">
+      <c r="B33" s="37"/>
+      <c r="C33" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" ht="16.5" spans="2:3">
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="35" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" ht="16.5" spans="2:3">
-      <c r="B35" s="21"/>
-      <c r="C35" s="18" t="s">
+      <c r="B35" s="37"/>
+      <c r="C35" s="35" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" ht="16.5" spans="2:3">
-      <c r="B36" s="21"/>
-      <c r="C36" s="18" t="s">
+      <c r="B36" s="37"/>
+      <c r="C36" s="35" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" ht="16.5" spans="2:3">
-      <c r="B37" s="21"/>
-      <c r="C37" s="20" t="s">
+      <c r="B37" s="37"/>
+      <c r="C37" s="36" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="38" ht="16.5" spans="2:3">
-      <c r="B38" s="21"/>
-      <c r="C38" s="18" t="s">
+      <c r="B38" s="37"/>
+      <c r="C38" s="35" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" ht="16.5" spans="2:3">
-      <c r="B39" s="21"/>
-      <c r="C39" s="18" t="s">
+      <c r="B39" s="37"/>
+      <c r="C39" s="35" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="40" ht="16.5" spans="2:3">
-      <c r="B40" s="21"/>
-      <c r="C40" s="18" t="s">
+      <c r="B40" s="37"/>
+      <c r="C40" s="35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" ht="16.5" spans="2:3">
-      <c r="B41" s="21"/>
-      <c r="C41" s="18" t="s">
+      <c r="B41" s="37"/>
+      <c r="C41" s="35" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" ht="16.5" spans="2:3">
-      <c r="B42" s="21"/>
-      <c r="C42" s="18" t="s">
+      <c r="B42" s="37"/>
+      <c r="C42" s="35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" ht="16.5" spans="2:3">
-      <c r="B43" s="21"/>
-      <c r="C43" s="18" t="s">
+      <c r="B43" s="37"/>
+      <c r="C43" s="35" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" ht="16.5" spans="2:3">
-      <c r="B44" s="21"/>
-      <c r="C44" s="18" t="s">
+      <c r="B44" s="37"/>
+      <c r="C44" s="35" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" ht="16.5" spans="2:3">
-      <c r="B45" s="21"/>
-      <c r="C45" s="18" t="s">
+      <c r="B45" s="37"/>
+      <c r="C45" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" ht="16.5" spans="2:3">
-      <c r="B46" s="21"/>
-      <c r="C46" s="18" t="s">
+      <c r="B46" s="37"/>
+      <c r="C46" s="35" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="47" ht="16.5" spans="2:3">
-      <c r="B47" s="21"/>
-      <c r="C47" s="18" t="s">
+      <c r="B47" s="37"/>
+      <c r="C47" s="35" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="48" ht="16.5" spans="2:3">
-      <c r="B48" s="21"/>
-      <c r="C48" s="18" t="s">
+      <c r="B48" s="37"/>
+      <c r="C48" s="35" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="49" ht="16.5" spans="2:3">
-      <c r="B49" s="21"/>
-      <c r="C49" s="18" t="s">
+      <c r="B49" s="37"/>
+      <c r="C49" s="35" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="50" ht="16.5" spans="2:3">
-      <c r="B50" s="21"/>
-      <c r="C50" s="18" t="s">
+      <c r="B50" s="37"/>
+      <c r="C50" s="35" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" ht="16.5" spans="2:3">
-      <c r="B51" s="21"/>
-      <c r="C51" s="18" t="s">
+      <c r="B51" s="37"/>
+      <c r="C51" s="35" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="52" ht="16.5" spans="2:3">
-      <c r="B52" s="21"/>
-      <c r="C52" s="18" t="s">
+      <c r="B52" s="37"/>
+      <c r="C52" s="35" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" ht="16.5" spans="2:3">
-      <c r="B53" s="21"/>
-      <c r="C53" s="18" t="s">
+      <c r="B53" s="37"/>
+      <c r="C53" s="35" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="54" ht="16.5" spans="2:3">
-      <c r="B54" s="21"/>
-      <c r="C54" s="18" t="s">
+      <c r="B54" s="37"/>
+      <c r="C54" s="35" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="55" ht="16.5" spans="2:3">
-      <c r="B55" s="21"/>
-      <c r="C55" s="18" t="s">
+      <c r="B55" s="37"/>
+      <c r="C55" s="35" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="56" ht="16.5" spans="2:3">
-      <c r="B56" s="21"/>
-      <c r="C56" s="18" t="s">
+      <c r="B56" s="37"/>
+      <c r="C56" s="35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="57" ht="16.5" spans="2:3">
-      <c r="B57" s="21"/>
-      <c r="C57" s="18" t="s">
+      <c r="B57" s="37"/>
+      <c r="C57" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="58" ht="16.5" spans="2:3">
-      <c r="B58" s="21"/>
-      <c r="C58" s="18" t="s">
+      <c r="B58" s="37"/>
+      <c r="C58" s="35" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="59" ht="16.5" spans="2:3">
-      <c r="B59" s="21"/>
-      <c r="C59" s="18" t="s">
+      <c r="B59" s="37"/>
+      <c r="C59" s="35" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="60" ht="16.5" spans="2:3">
-      <c r="B60" s="21"/>
-      <c r="C60" s="18" t="s">
+      <c r="B60" s="37"/>
+      <c r="C60" s="35" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="61" ht="16.5" spans="2:3">
-      <c r="B61" s="21"/>
-      <c r="C61" s="18" t="s">
+      <c r="B61" s="37"/>
+      <c r="C61" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="62" ht="16.5" spans="2:3">
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="35" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="63" ht="16.5" spans="2:3">
-      <c r="B63" s="21"/>
-      <c r="C63" s="18" t="s">
+      <c r="B63" s="37"/>
+      <c r="C63" s="35" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="64" ht="16.5" spans="2:3">
-      <c r="B64" s="21"/>
-      <c r="C64" s="18" t="s">
+      <c r="B64" s="37"/>
+      <c r="C64" s="35" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="65" ht="16.5" spans="2:3">
-      <c r="B65" s="21"/>
-      <c r="C65" s="18" t="s">
+      <c r="B65" s="37"/>
+      <c r="C65" s="35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="66" ht="16.5" spans="2:3">
-      <c r="B66" s="21"/>
-      <c r="C66" s="18" t="s">
+      <c r="B66" s="37"/>
+      <c r="C66" s="35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" ht="16.5" spans="2:3">
-      <c r="B67" s="21"/>
-      <c r="C67" s="18" t="s">
+      <c r="B67" s="37"/>
+      <c r="C67" s="35" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="68" ht="16.5" spans="2:3">
-      <c r="B68" s="21"/>
-      <c r="C68" s="18" t="s">
+      <c r="B68" s="37"/>
+      <c r="C68" s="35" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="69" ht="16.5" spans="2:3">
-      <c r="B69" s="21"/>
-      <c r="C69" s="18" t="s">
+      <c r="B69" s="37"/>
+      <c r="C69" s="35" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="70" ht="16.5" spans="2:3">
-      <c r="B70" s="21"/>
-      <c r="C70" s="18" t="s">
+      <c r="B70" s="37"/>
+      <c r="C70" s="35" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="71" ht="16.5" spans="2:3">
-      <c r="B71" s="21"/>
-      <c r="C71" s="18" t="s">
+      <c r="B71" s="37"/>
+      <c r="C71" s="35" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="72" ht="16.5" spans="2:3">
-      <c r="B72" s="21"/>
-      <c r="C72" s="18" t="s">
+      <c r="B72" s="37"/>
+      <c r="C72" s="35" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="73" ht="16.5" spans="2:3">
-      <c r="B73" s="21"/>
-      <c r="C73" s="18" t="s">
+      <c r="B73" s="37"/>
+      <c r="C73" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="74" ht="16.5" spans="2:3">
-      <c r="B74" s="21"/>
-      <c r="C74" s="18" t="s">
+      <c r="B74" s="37"/>
+      <c r="C74" s="35" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="75" ht="16.5" spans="2:3">
-      <c r="B75" s="21"/>
-      <c r="C75" s="18" t="s">
+      <c r="B75" s="37"/>
+      <c r="C75" s="35" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="76" ht="16.5" spans="2:3">
-      <c r="B76" s="21"/>
-      <c r="C76" s="18" t="s">
+      <c r="B76" s="37"/>
+      <c r="C76" s="35" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="77" ht="16.5" spans="2:3">
-      <c r="B77" s="21"/>
-      <c r="C77" s="18" t="s">
+      <c r="B77" s="37"/>
+      <c r="C77" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="78" ht="16.5" spans="2:3">
-      <c r="B78" s="21"/>
-      <c r="C78" s="18" t="s">
+      <c r="B78" s="37"/>
+      <c r="C78" s="35" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="79" ht="16.5" spans="2:3">
-      <c r="B79" s="21"/>
-      <c r="C79" s="18" t="s">
+      <c r="B79" s="37"/>
+      <c r="C79" s="35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="80" ht="16.5" spans="2:3">
-      <c r="B80" s="21"/>
-      <c r="C80" s="18" t="s">
+      <c r="B80" s="37"/>
+      <c r="C80" s="35" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="81" ht="16.5" spans="2:3">
-      <c r="B81" s="21"/>
-      <c r="C81" s="18" t="s">
+      <c r="B81" s="37"/>
+      <c r="C81" s="35" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="82" ht="16.5" spans="2:3">
-      <c r="B82" s="21"/>
-      <c r="C82" s="18" t="s">
+      <c r="B82" s="37"/>
+      <c r="C82" s="35" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="83" ht="16.5" spans="2:3">
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="C83" s="18" t="s">
+      <c r="C83" s="35" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="84" ht="16.5" spans="2:3">
-      <c r="B84" s="21"/>
-      <c r="C84" s="20" t="s">
+      <c r="B84" s="37"/>
+      <c r="C84" s="36" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="85" ht="16.5" spans="2:3">
-      <c r="B85" s="21"/>
-      <c r="C85" s="18" t="s">
+      <c r="B85" s="37"/>
+      <c r="C85" s="35" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="86" ht="16.5" spans="2:3">
-      <c r="B86" s="21"/>
-      <c r="C86" s="18" t="s">
+      <c r="B86" s="37"/>
+      <c r="C86" s="35" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="87" ht="16.5" spans="2:3">
-      <c r="B87" s="21"/>
-      <c r="C87" s="18" t="s">
+      <c r="B87" s="37"/>
+      <c r="C87" s="35" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="88" ht="16.5" spans="2:3">
-      <c r="B88" s="21"/>
-      <c r="C88" s="18" t="s">
+      <c r="B88" s="37"/>
+      <c r="C88" s="35" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="89" ht="16.5" spans="2:3">
-      <c r="B89" s="21"/>
-      <c r="C89" s="18" t="s">
+      <c r="B89" s="37"/>
+      <c r="C89" s="35" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="90" ht="16.5" spans="2:3">
-      <c r="B90" s="21"/>
-      <c r="C90" s="18" t="s">
+      <c r="B90" s="37"/>
+      <c r="C90" s="35" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="91" ht="16.5" spans="2:3">
-      <c r="B91" s="21"/>
-      <c r="C91" s="18" t="s">
+      <c r="B91" s="37"/>
+      <c r="C91" s="35" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="92" ht="16.5" spans="2:3">
-      <c r="B92" s="21"/>
-      <c r="C92" s="18" t="s">
+      <c r="B92" s="37"/>
+      <c r="C92" s="35" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="93" ht="16.5" spans="2:3">
-      <c r="B93" s="21"/>
-      <c r="C93" s="18" t="s">
+      <c r="B93" s="37"/>
+      <c r="C93" s="35" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="94" ht="16.5" spans="2:3">
-      <c r="B94" s="21"/>
-      <c r="C94" s="18" t="s">
+      <c r="B94" s="37"/>
+      <c r="C94" s="35" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="95" ht="16.5" spans="2:3">
-      <c r="B95" s="21"/>
-      <c r="C95" s="18" t="s">
+      <c r="B95" s="37"/>
+      <c r="C95" s="35" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="96" ht="16.5" spans="2:3">
-      <c r="B96" s="21"/>
-      <c r="C96" s="18" t="s">
+      <c r="B96" s="37"/>
+      <c r="C96" s="35" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="97" ht="16.5" spans="2:3">
-      <c r="B97" s="21"/>
-      <c r="C97" s="18" t="s">
+      <c r="B97" s="37"/>
+      <c r="C97" s="35" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="98" ht="16.5" spans="2:3">
-      <c r="B98" s="21"/>
-      <c r="C98" s="18" t="s">
+      <c r="B98" s="37"/>
+      <c r="C98" s="35" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="99" ht="16.5" spans="2:3">
-      <c r="B99" s="21"/>
-      <c r="C99" s="18" t="s">
+      <c r="B99" s="37"/>
+      <c r="C99" s="35" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="100" ht="16.5" spans="2:3">
-      <c r="B100" s="21"/>
-      <c r="C100" s="18" t="s">
+      <c r="B100" s="37"/>
+      <c r="C100" s="35" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="101" ht="16.5" spans="2:3">
-      <c r="B101" s="21"/>
-      <c r="C101" s="18" t="s">
+      <c r="B101" s="37"/>
+      <c r="C101" s="35" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="102" ht="16.5" spans="2:3">
-      <c r="B102" s="21"/>
-      <c r="C102" s="18" t="s">
+      <c r="B102" s="37"/>
+      <c r="C102" s="35" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="103" ht="16.5" spans="2:3">
-      <c r="B103" s="21"/>
-      <c r="C103" s="18" t="s">
+      <c r="B103" s="37"/>
+      <c r="C103" s="35" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="104" ht="16.5" spans="2:3">
-      <c r="B104" s="21" t="s">
+      <c r="B104" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C104" s="18" t="s">
+      <c r="C104" s="35" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="105" ht="16.5" spans="2:3">
-      <c r="B105" s="21"/>
-      <c r="C105" s="18" t="s">
+      <c r="B105" s="37"/>
+      <c r="C105" s="35" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="106" ht="16.5" spans="2:3">
-      <c r="B106" s="21" t="s">
+      <c r="B106" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="18" t="s">
+      <c r="C106" s="35" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="107" ht="16.5" spans="2:3">
-      <c r="B107" s="21"/>
-      <c r="C107" s="18" t="s">
+      <c r="B107" s="37"/>
+      <c r="C107" s="35" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="108" ht="16.5" spans="2:3">
-      <c r="B108" s="21"/>
-      <c r="C108" s="18" t="s">
+      <c r="B108" s="37"/>
+      <c r="C108" s="35" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="109" ht="16.5" spans="2:3">
-      <c r="B109" s="21"/>
-      <c r="C109" s="18" t="s">
+      <c r="B109" s="37"/>
+      <c r="C109" s="35" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="110" ht="16.5" spans="2:3">
-      <c r="B110" s="21"/>
-      <c r="C110" s="18" t="s">
+      <c r="B110" s="37"/>
+      <c r="C110" s="35" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="111" ht="16.5" spans="2:3">
-      <c r="B111" s="21"/>
-      <c r="C111" s="18" t="s">
+      <c r="B111" s="37"/>
+      <c r="C111" s="35" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="112" ht="16.5" spans="2:3">
-      <c r="B112" s="21"/>
-      <c r="C112" s="18" t="s">
+      <c r="B112" s="37"/>
+      <c r="C112" s="35" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3038,1200 +3335,1200 @@
   <sheetPr/>
   <dimension ref="B1:J105"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B94" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.6666666666667" style="2" customWidth="1"/>
-    <col min="5" max="5" width="37.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.66666666666667" style="2" customWidth="1"/>
-    <col min="7" max="7" width="58.5833333333333" style="2" customWidth="1"/>
-    <col min="8" max="12" width="9" style="2"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="18"/>
+    <col min="2" max="2" width="14" style="19" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="19" customWidth="1"/>
+    <col min="4" max="4" width="18.6666666666667" style="19" customWidth="1"/>
+    <col min="5" max="5" width="37.5" style="19" customWidth="1"/>
+    <col min="6" max="6" width="4.66666666666667" style="19" customWidth="1"/>
+    <col min="7" max="7" width="58.5833333333333" style="19" customWidth="1"/>
+    <col min="8" max="12" width="9" style="19"/>
+    <col min="13" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:7">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="20">
         <v>1988</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20">
         <v>1993</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="20" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20">
         <v>1999</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20">
         <v>2004</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="20" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20">
         <v>2018</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="G10" s="3" t="s">
+      <c r="E10" s="20"/>
+      <c r="G10" s="20" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="G11" s="3" t="s">
+      <c r="E11" s="20"/>
+      <c r="G11" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2" t="s">
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="19" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="10" t="s">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="3" t="s">
+      <c r="F25" s="28"/>
+      <c r="G25" s="20" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="3"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="3"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="3"/>
-      <c r="C38" s="3" t="s">
+      <c r="B38" s="20"/>
+      <c r="C38" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="20" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="3" t="s">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3" t="s">
+      <c r="F39" s="20"/>
+      <c r="G39" s="20" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="3" t="s">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3" t="s">
+      <c r="F40" s="20"/>
+      <c r="G40" s="20" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="3" t="s">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3" t="s">
+      <c r="F41" s="20"/>
+      <c r="G41" s="20" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3" t="s">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3" t="s">
+      <c r="F42" s="20"/>
+      <c r="G42" s="20" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3" t="s">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3" t="s">
+      <c r="F43" s="20"/>
+      <c r="G43" s="20" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3" t="s">
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3" t="s">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3" t="s">
+      <c r="F47" s="20"/>
+      <c r="G47" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3" t="s">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3" t="s">
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3" t="s">
+      <c r="F50" s="20"/>
+      <c r="G50" s="20" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3" t="s">
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3" t="s">
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3" t="s">
+      <c r="F54" s="20"/>
+      <c r="G54" s="20" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3" t="s">
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3" t="s">
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3" t="s">
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3" t="s">
+      <c r="F57" s="20"/>
+      <c r="G57" s="20" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3" t="s">
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3" t="s">
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3" t="s">
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3" t="s">
+      <c r="F60" s="20"/>
+      <c r="G60" s="20" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3" t="s">
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3" t="s">
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3" t="s">
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3" t="s">
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3" t="s">
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3" t="s">
+      <c r="F65" s="20"/>
+      <c r="G65" s="20" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3" t="s">
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3" t="s">
+      <c r="F66" s="20"/>
+      <c r="G66" s="20" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3" t="s">
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="3"/>
-      <c r="C68" s="4" t="s">
+      <c r="B68" s="20"/>
+      <c r="C68" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3" t="s">
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="3"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="3" t="s">
+      <c r="B69" s="20"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
     </row>
     <row r="70" spans="2:7">
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
     </row>
     <row r="72" spans="2:7">
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4" t="s">
+      <c r="D72" s="21"/>
+      <c r="E72" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="14"/>
-      <c r="C73" s="15" t="s">
+      <c r="B73" s="31"/>
+      <c r="C73" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E73" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3" t="s">
+      <c r="F73" s="20"/>
+      <c r="G73" s="20" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="14"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="3" t="s">
+      <c r="B74" s="31"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
+      <c r="E74" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3" t="s">
+      <c r="F74" s="20"/>
+      <c r="G74" s="20" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="14"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="3" t="s">
+      <c r="B75" s="31"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3" t="s">
+      <c r="F75" s="20"/>
+      <c r="G75" s="20" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="76" spans="2:7">
-      <c r="B76" s="14"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="3" t="s">
+      <c r="B76" s="31"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3" t="s">
+      <c r="F76" s="20"/>
+      <c r="G76" s="20" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="77" spans="2:7">
-      <c r="B77" s="14"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="3" t="s">
+      <c r="B77" s="31"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
     </row>
     <row r="78" spans="2:7">
-      <c r="B78" s="14"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="3" t="s">
+      <c r="B78" s="31"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3" t="s">
+      <c r="F78" s="20"/>
+      <c r="G78" s="20" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="79" spans="2:7">
-      <c r="B79" s="14"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="3" t="s">
+      <c r="B79" s="31"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
+      <c r="E79" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="14"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="3" t="s">
+      <c r="B80" s="31"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
+      <c r="E80" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="16"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="3" t="s">
+      <c r="B81" s="33"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="C82" s="16" t="s">
+      <c r="C82" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="D82" s="16"/>
-      <c r="E82" s="6" t="s">
+      <c r="D82" s="33"/>
+      <c r="E82" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="15"/>
-      <c r="C83" s="15" t="s">
+      <c r="B83" s="32"/>
+      <c r="C83" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E83" s="3" t="s">
+      <c r="E83" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="15"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="3" t="s">
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="15"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="3" t="s">
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="32"/>
+      <c r="E85" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="15"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="3" t="s">
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="32"/>
+      <c r="E86" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
     </row>
     <row r="87" spans="2:7">
-      <c r="B87" s="15"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="3" t="s">
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="32"/>
+      <c r="E87" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="20"/>
     </row>
     <row r="88" spans="2:7">
-      <c r="B88" s="15"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="3" t="s">
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="32"/>
+      <c r="E88" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="20"/>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" s="15"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="3" t="s">
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="32"/>
+      <c r="E89" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
     </row>
     <row r="90" spans="2:7">
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="3" t="s">
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3" t="s">
+      <c r="F90" s="20"/>
+      <c r="G90" s="20" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="91" spans="2:7">
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="C91" s="6" t="s">
+      <c r="C91" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6" t="s">
+      <c r="D91" s="23"/>
+      <c r="E91" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
     </row>
     <row r="92" spans="2:7">
-      <c r="B92" s="15"/>
-      <c r="C92" s="15" t="s">
+      <c r="B92" s="32"/>
+      <c r="C92" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E92" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="20"/>
     </row>
     <row r="93" spans="2:7">
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="3" t="s">
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="32"/>
+      <c r="E93" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
     </row>
     <row r="94" spans="2:7">
-      <c r="B94" s="15"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="3" t="s">
+      <c r="B94" s="32"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="32"/>
+      <c r="E94" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
     </row>
     <row r="95" spans="2:7">
-      <c r="B95" s="15"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="3" t="s">
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3" t="s">
+      <c r="F95" s="20"/>
+      <c r="G95" s="20" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="96" spans="2:7">
-      <c r="B96" s="15"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="3" t="s">
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3" t="s">
+      <c r="F96" s="20"/>
+      <c r="G96" s="20" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="97" spans="2:7">
-      <c r="B97" s="15"/>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="3" t="s">
+      <c r="B97" s="32"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
     </row>
     <row r="98" spans="2:7">
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="33" t="s">
         <v>273</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="C98" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6" t="s">
+      <c r="D98" s="23"/>
+      <c r="E98" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
     </row>
     <row r="99" spans="2:7">
-      <c r="B99" s="15"/>
-      <c r="C99" s="15" t="s">
+      <c r="B99" s="32"/>
+      <c r="C99" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="D99" s="15" t="s">
+      <c r="D99" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E99" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="20"/>
     </row>
     <row r="100" spans="2:7">
-      <c r="B100" s="15"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="15"/>
-      <c r="E100" s="3" t="s">
+      <c r="B100" s="32"/>
+      <c r="C100" s="32"/>
+      <c r="D100" s="32"/>
+      <c r="E100" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="20"/>
     </row>
     <row r="101" spans="2:7">
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
-      <c r="D101" s="15"/>
-      <c r="E101" s="3" t="s">
+      <c r="B101" s="32"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3" t="s">
+      <c r="F101" s="20"/>
+      <c r="G101" s="20" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="102" spans="2:7">
-      <c r="B102" s="15"/>
-      <c r="C102" s="15"/>
-      <c r="D102" s="15"/>
-      <c r="E102" s="3" t="s">
+      <c r="B102" s="32"/>
+      <c r="C102" s="32"/>
+      <c r="D102" s="32"/>
+      <c r="E102" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="20"/>
     </row>
     <row r="103" spans="2:7">
-      <c r="B103" s="15"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="3" t="s">
+      <c r="B103" s="32"/>
+      <c r="C103" s="32"/>
+      <c r="D103" s="32"/>
+      <c r="E103" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3" t="s">
+      <c r="F103" s="20"/>
+      <c r="G103" s="20" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="104" spans="2:7">
-      <c r="B104" s="15"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="3" t="s">
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
     </row>
     <row r="105" spans="2:7">
-      <c r="B105" s="15"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="3" t="s">
+      <c r="B105" s="32"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="20" t="s">
         <v>284</v>
       </c>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3" t="s">
+      <c r="F105" s="20"/>
+      <c r="G105" s="20" t="s">
         <v>285</v>
       </c>
     </row>
@@ -4282,7 +4579,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="4" spans="4:4">
       <c r="D4" t="s">
@@ -4293,4 +4590,522 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="16384" width="8.66666666666667" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2"/>
+      <c r="B6" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="2"/>
+      <c r="B19" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="46">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="A1:A32"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C2:D3"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="D21:F24"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>